<commit_message>
Added P02_1, P04_8, P09_4, P18_2, P20_1
</commit_message>
<xml_diff>
--- a/analysis/mails_01/P16_1/table_to_fill.xlsx
+++ b/analysis/mails_01/P16_1/table_to_fill.xlsx
@@ -670,19 +670,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -710,7 +710,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -750,19 +750,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -770,7 +770,9 @@
       <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
       <c r="I5" t="s">
         <v>21</v>
       </c>
@@ -790,25 +792,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" t="s">
@@ -821,28 +823,30 @@
         <v>23</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="M6" t="s">
+        <v>42</v>
+      </c>
       <c r="N6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -870,29 +874,27 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" t="s">
-        <v>35</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H8" s="2"/>
       <c r="I8" t="s">
         <v>21</v>
       </c>
@@ -903,38 +905,38 @@
         <v>23</v>
       </c>
       <c r="L8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="M8" t="s">
+        <v>51</v>
+      </c>
       <c r="N8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
         <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>35</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="H9" s="2"/>
       <c r="I9" t="s">
         <v>21</v>
       </c>
@@ -945,34 +947,36 @@
         <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="M9" t="s">
+        <v>42</v>
+      </c>
       <c r="N9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" t="s">
@@ -988,383 +992,9 @@
         <v>41</v>
       </c>
       <c r="M10" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" t="s">
-        <v>42</v>
-      </c>
-      <c r="N11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="3"/>
-      <c r="N12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="3"/>
-      <c r="N13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" t="s">
-        <v>41</v>
-      </c>
-      <c r="M14" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" t="s">
-        <v>41</v>
-      </c>
-      <c r="M15" t="s">
-        <v>51</v>
-      </c>
-      <c r="N15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" t="s">
-        <v>41</v>
-      </c>
-      <c r="M16" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" t="s">
-        <v>42</v>
-      </c>
-      <c r="N17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" t="s">
-        <v>41</v>
-      </c>
-      <c r="M18" t="s">
-        <v>55</v>
-      </c>
-      <c r="N18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" t="s">
-        <v>41</v>
-      </c>
-      <c r="M19" t="s">
-        <v>55</v>
-      </c>
-      <c r="N19" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>